<commit_message>
📝 ajout des équivalents ports GPIO
</commit_message>
<xml_diff>
--- a/Nouveau PIR/docs/continental/port_mapping.xlsx
+++ b/Nouveau PIR/docs/continental/port_mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Cours\PIR\PIR\Nouveau PIR\docs\continental\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{384DACF5-6166-4D24-8049-1C0A1289A436}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4353313-F8A4-4B88-AC97-D0BDD3FE79DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -205,7 +205,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -248,6 +248,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="16">
     <border>
@@ -480,7 +486,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -504,6 +510,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -787,7 +794,7 @@
   <dimension ref="A1:P20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -864,21 +871,27 @@
       <c r="F3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="8"/>
+      <c r="G3" s="23">
+        <v>0</v>
+      </c>
       <c r="H3" s="22" t="s">
         <v>16</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="J3" s="8"/>
+      <c r="J3" s="23">
+        <v>4</v>
+      </c>
       <c r="K3" s="22" t="s">
         <v>15</v>
       </c>
       <c r="L3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="M3" s="8"/>
+      <c r="M3" s="23">
+        <v>7</v>
+      </c>
       <c r="N3" s="21"/>
       <c r="O3" s="21"/>
       <c r="P3" s="21"/>
@@ -896,21 +909,27 @@
       <c r="F4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="8"/>
+      <c r="G4" s="23">
+        <v>1</v>
+      </c>
       <c r="H4" s="22" t="s">
         <v>17</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="J4" s="8"/>
+      <c r="J4" s="23">
+        <v>5</v>
+      </c>
       <c r="K4" s="22" t="s">
         <v>32</v>
       </c>
       <c r="L4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="M4" s="8"/>
+      <c r="M4" s="23">
+        <v>8</v>
+      </c>
       <c r="N4" s="21"/>
       <c r="O4" s="21"/>
       <c r="P4" s="21"/>
@@ -928,21 +947,27 @@
       <c r="F5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="8"/>
+      <c r="G5" s="23">
+        <v>2</v>
+      </c>
       <c r="H5" s="22" t="s">
         <v>18</v>
       </c>
       <c r="I5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="J5" s="8"/>
+      <c r="J5" s="23">
+        <v>6</v>
+      </c>
       <c r="K5" s="22" t="s">
         <v>13</v>
       </c>
       <c r="L5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="M5" s="8"/>
+      <c r="M5" s="23">
+        <v>9</v>
+      </c>
       <c r="N5" s="21"/>
       <c r="O5" s="21"/>
       <c r="P5" s="21"/>
@@ -960,7 +985,9 @@
       <c r="F6" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="G6" s="8"/>
+      <c r="G6" s="23">
+        <v>3</v>
+      </c>
       <c r="H6" s="7"/>
       <c r="I6" s="2"/>
       <c r="J6" s="8"/>
@@ -970,7 +997,9 @@
       <c r="L6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="M6" s="8"/>
+      <c r="M6" s="23">
+        <v>10</v>
+      </c>
       <c r="N6" s="21"/>
       <c r="O6" s="21"/>
       <c r="P6" s="21"/>
@@ -994,7 +1023,9 @@
       <c r="L7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M7" s="8"/>
+      <c r="M7" s="23">
+        <v>11</v>
+      </c>
       <c r="N7" s="21"/>
       <c r="O7" s="21"/>
       <c r="P7" s="21"/>
@@ -1018,7 +1049,9 @@
       <c r="L8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="M8" s="8"/>
+      <c r="M8" s="23">
+        <v>12</v>
+      </c>
       <c r="N8" s="21"/>
       <c r="O8" s="21"/>
       <c r="P8" s="21"/>

</xml_diff>